<commit_message>
Excel convert Json 작업 중
</commit_message>
<xml_diff>
--- a/Share/ExcelTemplate/UserGroup.xlsx
+++ b/Share/ExcelTemplate/UserGroup.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trim0\Documents\source\Handy\Share\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trim0\Documents\source\Handy\Share\ExcelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365359DC-0A4A-4880-B65E-92F2F98D51CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23C1EB7-7C7C-4E4B-A2C1-9ACA8EA181D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6800" yWindow="2420" windowWidth="21660" windowHeight="8370" activeTab="1" xr2:uid="{6ADC8A4A-52FB-4BCF-AD8C-6ABEE9BA9AC6}"/>
+    <workbookView xWindow="2150" yWindow="1410" windowWidth="21660" windowHeight="8370" activeTab="1" xr2:uid="{6ADC8A4A-52FB-4BCF-AD8C-6ABEE9BA9AC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -70,6 +70,10 @@
   </si>
   <si>
     <t>User</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dummy</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -116,8 +120,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -434,36 +441,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4098C1E5-3B7A-417D-BD26-98193AB53BA8}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -475,10 +500,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CCA3CBB-575C-4053-A3D1-EBA33DD6A464}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -525,6 +550,20 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Excel To Json 커밋
</commit_message>
<xml_diff>
--- a/Share/ExcelTemplate/UserGroup.xlsx
+++ b/Share/ExcelTemplate/UserGroup.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trim0\Documents\source\Kosher\Share\ExcelTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76211CCE-2DEA-42A0-A188-E5CBE9B0A6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACFA045-2E77-4744-AD35-AEBEF47AE03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7280" yWindow="3160" windowWidth="17940" windowHeight="8210" activeTab="1" xr2:uid="{6ADC8A4A-52FB-4BCF-AD8C-6ABEE9BA9AC6}"/>
+    <workbookView xWindow="1520" yWindow="6540" windowWidth="17940" windowHeight="8210" xr2:uid="{6ADC8A4A-52FB-4BCF-AD8C-6ABEE9BA9AC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -100,15 +100,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>object</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Test</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>TEst123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>class</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4098C1E5-3B7A-417D-BD26-98193AB53BA8}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -526,7 +526,10 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="F3">
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -543,7 +546,10 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="F4">
+        <v>1443</v>
       </c>
     </row>
   </sheetData>
@@ -557,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CCA3CBB-575C-4053-A3D1-EBA33DD6A464}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -630,7 +636,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>1</v>

</xml_diff>